<commit_message>
update for latest magnets
</commit_message>
<xml_diff>
--- a/demo_parameters.xlsx
+++ b/demo_parameters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t xml:space="preserve">Cooling Cell Parameters</t>
   </si>
@@ -154,31 +154,46 @@
     <t xml:space="preserve">Field</t>
   </si>
   <si>
+    <t xml:space="preserve">Coil 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dipole z centre position</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coil inner radius</t>
   </si>
   <si>
-    <t xml:space="preserve">Dipole z centre position</t>
+    <t xml:space="preserve">Dipole field direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical</t>
   </si>
   <si>
     <t xml:space="preserve">Coil length</t>
   </si>
   <si>
-    <t xml:space="preserve">Dipole field direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertical</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coil radial thickness</t>
   </si>
   <si>
     <t xml:space="preserve">Coil z centre position</t>
   </si>
   <si>
+    <t xml:space="preserve">Pancake length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spacer length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number pancakes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Current Density</t>
   </si>
   <si>
     <t xml:space="preserve">A/mm^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coil 2</t>
   </si>
   <si>
     <t xml:space="preserve">*Solenoid field on axis defined by B = B0.5 sin( pi z/L) + B0 sin(2 pi z/L) + B1 sin(4 pi z/L) + B2 sin (6 pi z/L)</t>
@@ -224,7 +239,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +264,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF38"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -284,7 +305,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -310,6 +331,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -337,7 +366,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -398,16 +427,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.78"/>
   </cols>
   <sheetData>
@@ -581,8 +610,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="6" t="n">
-        <f aca="false">7/0.8</f>
-        <v>8.75</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>22</v>
@@ -599,8 +627,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="6" t="n">
-        <f aca="false">1/0.8</f>
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>22</v>
@@ -640,7 +667,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="6" t="n">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>6</v>
@@ -754,15 +781,11 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="6" t="n">
-        <v>250</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6" t="s">
         <v>45</v>
@@ -779,7 +802,7 @@
         <v>46</v>
       </c>
       <c r="B22" s="6" t="n">
-        <v>140</v>
+        <v>285</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>6</v>
@@ -797,8 +820,8 @@
       <c r="A23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="7" t="n">
-        <v>169.3</v>
+      <c r="B23" s="6" t="n">
+        <v>268</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>6</v>
@@ -812,8 +835,8 @@
       <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="7" t="n">
-        <v>100.7</v>
+      <c r="B24" s="9" t="n">
+        <v>70</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>6</v>
@@ -827,11 +850,11 @@
       <c r="A25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="6" t="n">
-        <v>500</v>
+      <c r="B25" s="9" t="n">
+        <v>211</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -839,41 +862,164 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="A26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="C28" s="6"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="6" t="n">
+        <v>328.43</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="8"/>
+      <c r="A30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="6" t="n">
+        <v>185</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="E31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="6" t="n">
+        <v>72</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="9" t="n">
+        <v>81</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="6" t="n">
+        <v>300</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>